<commit_message>
exports all new patients now
</commit_message>
<xml_diff>
--- a/Data csv/Patients 10:22:23.xlsx
+++ b/Data csv/Patients 10:22:23.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H839"/>
+  <dimension ref="A1:H858"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -27288,6 +27288,669 @@
         </is>
       </c>
     </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>Anaudia Johnson</t>
+        </is>
+      </c>
+      <c r="B840" s="2">
+        <v>45221</v>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D840" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E840">
+        <v>24.28523515198806</v>
+      </c>
+      <c r="F840" s="2">
+        <v>36351</v>
+      </c>
+      <c r="G840" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>Barney rogers</t>
+        </is>
+      </c>
+      <c r="B841" s="2">
+        <v>45223</v>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D841" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="E841">
+        <v>999</v>
+      </c>
+      <c r="F841" s="2">
+        <v>-306287</v>
+      </c>
+      <c r="G841" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H841" t="inlineStr">
+        <is>
+          <t>27503</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>Denisha Smith</t>
+        </is>
+      </c>
+      <c r="B842" s="2">
+        <v>45224</v>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D842" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E842">
+        <v>24.95864619624861</v>
+      </c>
+      <c r="F842" s="2">
+        <v>36108</v>
+      </c>
+      <c r="G842" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H842" t="inlineStr">
+        <is>
+          <t>27707</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>Carla Green</t>
+        </is>
+      </c>
+      <c r="B843" s="2">
+        <v>45227</v>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D843" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E843">
+        <v>34.36073293770577</v>
+      </c>
+      <c r="F843" s="2">
+        <v>32677</v>
+      </c>
+      <c r="G843" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H843" t="inlineStr">
+        <is>
+          <t>27707</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>Emily Harrington</t>
+        </is>
+      </c>
+      <c r="B844" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D844" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E844">
+        <v>22.7683205906578</v>
+      </c>
+      <c r="F844" s="2">
+        <v>36914</v>
+      </c>
+      <c r="G844" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H844" t="inlineStr">
+        <is>
+          <t>27519</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>Deborah Chapman</t>
+        </is>
+      </c>
+      <c r="B845" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D845" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E845">
+        <v>56.75396026840615</v>
+      </c>
+      <c r="F845" s="2">
+        <v>24501</v>
+      </c>
+      <c r="G845" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H845" t="inlineStr">
+        <is>
+          <t>27701</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>Cynthia Parrish Fox</t>
+        </is>
+      </c>
+      <c r="B846" s="2">
+        <v>45230</v>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D846" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E846">
+        <v>67.29501632477053</v>
+      </c>
+      <c r="F846" s="2">
+        <v>20651</v>
+      </c>
+      <c r="G846" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H846" t="inlineStr">
+        <is>
+          <t>27707</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>Ja'Naise Allison</t>
+        </is>
+      </c>
+      <c r="B847" s="2">
+        <v>45232</v>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D847" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E847">
+        <v>0.7226933703863415</v>
+      </c>
+      <c r="F847" s="2">
+        <v>44968</v>
+      </c>
+      <c r="G847" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H847" t="inlineStr">
+        <is>
+          <t>27701</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>Sandra McGhee-Bureh</t>
+        </is>
+      </c>
+      <c r="B848" s="2">
+        <v>45235</v>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D848" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E848">
+        <v>67.61797527213655</v>
+      </c>
+      <c r="F848" s="2">
+        <v>20538</v>
+      </c>
+      <c r="G848" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H848" t="inlineStr">
+        <is>
+          <t>27603</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>Jean McGhee</t>
+        </is>
+      </c>
+      <c r="B849" s="2">
+        <v>45235</v>
+      </c>
+      <c r="D849" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E849">
+        <v>0</v>
+      </c>
+      <c r="F849" s="2">
+        <v>45235</v>
+      </c>
+      <c r="G849" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H849" t="inlineStr">
+        <is>
+          <t>27573</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>Deborah E. Baker</t>
+        </is>
+      </c>
+      <c r="B850" s="2">
+        <v>45235</v>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D850" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E850">
+        <v>67.20466539353991</v>
+      </c>
+      <c r="F850" s="2">
+        <v>20689</v>
+      </c>
+      <c r="G850" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H850" t="inlineStr">
+        <is>
+          <t>27217</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>Juan de Dios Argueta</t>
+        </is>
+      </c>
+      <c r="B851" s="2">
+        <v>45236</v>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="D851" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="E851">
+        <v>24.33189365056549</v>
+      </c>
+      <c r="F851" s="2">
+        <v>36349</v>
+      </c>
+      <c r="G851" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H851" t="inlineStr">
+        <is>
+          <t>27701</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>Waleed Razzaq</t>
+        </is>
+      </c>
+      <c r="B852" s="2">
+        <v>45238</v>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D852" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="E852">
+        <v>60.74320485704703</v>
+      </c>
+      <c r="F852" s="2">
+        <v>23052</v>
+      </c>
+      <c r="G852" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H852" t="inlineStr">
+        <is>
+          <t>27893</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>Sandra McFadgir</t>
+        </is>
+      </c>
+      <c r="B853" s="2">
+        <v>45238</v>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D853" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E853">
+        <v>61.95609766114294</v>
+      </c>
+      <c r="F853" s="2">
+        <v>22609</v>
+      </c>
+      <c r="G853" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H853" t="inlineStr">
+        <is>
+          <t>27703</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>Vickie Bailey</t>
+        </is>
+      </c>
+      <c r="B854" s="2">
+        <v>45238</v>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D854" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E854">
+        <v>58.93618623243461</v>
+      </c>
+      <c r="F854" s="2">
+        <v>23712</v>
+      </c>
+      <c r="G854" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>Karen Richard</t>
+        </is>
+      </c>
+      <c r="B855" s="2">
+        <v>45242</v>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D855" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E855">
+        <v>67.82617028412631</v>
+      </c>
+      <c r="F855" s="2">
+        <v>20469</v>
+      </c>
+      <c r="G855" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H855" t="inlineStr">
+        <is>
+          <t>27574</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>Brian Long</t>
+        </is>
+      </c>
+      <c r="B856" s="2">
+        <v>45244</v>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D856" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="E856">
+        <v>53.87927199052684</v>
+      </c>
+      <c r="F856" s="2">
+        <v>25565</v>
+      </c>
+      <c r="G856" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H856" t="inlineStr">
+        <is>
+          <t>27703</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>linda Hunter</t>
+        </is>
+      </c>
+      <c r="B857" s="2">
+        <v>45244</v>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>Black, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D857" t="inlineStr">
+        <is>
+          <t>Woman</t>
+        </is>
+      </c>
+      <c r="E857">
+        <v>35.96788435080803</v>
+      </c>
+      <c r="F857" s="2">
+        <v>32107</v>
+      </c>
+      <c r="G857" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H857" t="inlineStr">
+        <is>
+          <t>27513</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>Bryce Bates</t>
+        </is>
+      </c>
+      <c r="B858" s="2">
+        <v>45244</v>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>White, Not Hispanic</t>
+        </is>
+      </c>
+      <c r="D858" t="inlineStr">
+        <is>
+          <t>Man</t>
+        </is>
+      </c>
+      <c r="G858" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="H858" t="inlineStr">
+        <is>
+          <t>27705</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>